<commit_message>
Updated ZAF model - 2025-07-29 14:55
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/SysSettings.xlsx
+++ b/VerveStacks_ZAF/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA12D0FF-53EE-4591-ABE0-C3E355A6A4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D746323-F86F-4287-B7DA-8121F9D1CCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="system_settings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="216">
   <si>
     <t>~BookRegions_Map</t>
   </si>
@@ -680,6 +680,9 @@
   </si>
   <si>
     <t>electricity used in road transport</t>
+  </si>
+  <si>
+    <t>NCAP_AF</t>
   </si>
   <si>
     <t>ZAF</t>
@@ -3058,7 +3061,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -3085,7 +3088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F298A9-BCD9-4ABF-BE3B-9D1BDD3E7001}">
   <dimension ref="B3:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -3609,10 +3612,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A64C410-895F-4040-A7AB-3F7211AA7FBD}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="11.65"/>
@@ -3729,49 +3732,49 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="14" t="s">
+    <row r="9" spans="1:11">
+      <c r="C9" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="15" t="s">
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B13" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C13" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D13" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E13" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F13" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G13" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H13" s="15" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="C13" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="11">
-        <v>2222</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -3779,22 +3782,22 @@
         <v>70</v>
       </c>
       <c r="E14" s="11">
+        <v>2222</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="C15" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="11">
         <v>8888</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="12.75">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:11" ht="12.75">
       <c r="A16" s="13"/>
@@ -3819,9 +3822,7 @@
       <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:13" ht="12.75">
-      <c r="A18" s="13" t="s">
-        <v>73</v>
-      </c>
+      <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -3833,62 +3834,64 @@
     </row>
     <row r="19" spans="1:13" ht="12.75">
       <c r="A19" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>79</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:13" ht="14.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:13" ht="12.75">
+      <c r="A20" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:13" ht="14.25">
+      <c r="A21" t="s">
         <v>208</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>211</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>209</v>
       </c>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20" t="s">
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21" t="s">
         <v>210</v>
       </c>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-    </row>
-    <row r="21" spans="1:13" ht="12.75">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
     </row>
     <row r="22" spans="1:13" ht="12.75">
       <c r="A22" s="13"/>
@@ -3912,20 +3915,16 @@
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:13" ht="14.25">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
+    <row r="24" spans="1:13" ht="12.75">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
     </row>
     <row r="25" spans="1:13" ht="14.25">
       <c r="A25"/>
@@ -4151,6 +4150,21 @@
       <c r="K39"/>
       <c r="L39"/>
       <c r="M39"/>
+    </row>
+    <row r="40" spans="1:13" ht="14.25">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>